<commit_message>
ALTERAÇÃO NOMES DE COLUNAS
</commit_message>
<xml_diff>
--- a/Producao/Modelos/PROGRAMACAO_PROGRAMACAO_MODELO.xlsx
+++ b/Producao/Modelos/PROGRAMACAO_PROGRAMACAO_MODELO.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Source\Repos\wognascimento\SIG\SIG\Producao\Producao\Modelos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CIPOLATTI\SISTEMAS\Producao\Producao\Modelos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E21FC89D-7D7E-473A-A3F2-E8082AC39181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC50DD19-09CB-495F-B16C-5D925805548C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{D9A668C6-916A-46D2-B14A-67ECE735CF5F}"/>
+    <workbookView xWindow="38280" yWindow="-1110" windowWidth="38640" windowHeight="15720" xr2:uid="{D9A668C6-916A-46D2-B14A-67ECE735CF5F}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -41,12 +41,6 @@
     <t>PROGRAMAÇÃO DE PRODUÇÃO</t>
   </si>
   <si>
-    <t>ENCARREGADO:</t>
-  </si>
-  <si>
-    <t>RESPONSAVEL:</t>
-  </si>
-  <si>
     <t>FILA/M.O:</t>
   </si>
   <si>
@@ -105,6 +99,12 @@
   </si>
   <si>
     <t>ORD</t>
+  </si>
+  <si>
+    <t>PLANILHAS:</t>
+  </si>
+  <si>
+    <t>SETOR:</t>
   </si>
 </sst>
 </file>
@@ -232,6 +232,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -246,12 +252,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -271,9 +271,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office 2013 - 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -311,7 +311,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -417,7 +417,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -559,7 +559,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -570,7 +570,7 @@
   <dimension ref="B1:T8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="F5" sqref="F5:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -594,45 +594,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:20" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="B1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
+      <c r="B1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
     </row>
     <row r="3" spans="2:20" x14ac:dyDescent="0.25">
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
-      <c r="K3" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="L3" s="7"/>
-      <c r="M3" s="8"/>
+      <c r="K3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="L3" s="9"/>
+      <c r="M3" s="10"/>
       <c r="N3" s="1">
         <f>COUNTIF(N9:N1048576,"FILA/M.O")</f>
         <v>0</v>
       </c>
-      <c r="O3" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="P3" s="7"/>
-      <c r="Q3" s="8"/>
+      <c r="O3" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="P3" s="9"/>
+      <c r="Q3" s="10"/>
       <c r="R3" s="1">
         <f>COUNTIF(N9:N1048576,"INDEFINIDO")</f>
         <v>0</v>
@@ -641,27 +641,27 @@
     <row r="4" spans="2:20" x14ac:dyDescent="0.25">
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
-      <c r="F4" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="G4" s="8"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="L4" s="7"/>
-      <c r="M4" s="8"/>
+      <c r="F4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="10"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="L4" s="9"/>
+      <c r="M4" s="10"/>
       <c r="N4" s="1">
         <f>COUNTIF(N9:N1048576,"EM ANDAMENTO")</f>
         <v>0</v>
       </c>
-      <c r="O4" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="P4" s="7"/>
-      <c r="Q4" s="8"/>
+      <c r="O4" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="P4" s="9"/>
+      <c r="Q4" s="10"/>
       <c r="R4" s="1">
         <f>COUNTIF(N9:N1048576,"PROJETOS")</f>
         <v>0</v>
@@ -670,27 +670,27 @@
     <row r="5" spans="2:20" x14ac:dyDescent="0.25">
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
-      <c r="F5" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="G5" s="8"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="L5" s="7"/>
-      <c r="M5" s="8"/>
+      <c r="F5" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="10"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="L5" s="9"/>
+      <c r="M5" s="10"/>
       <c r="N5" s="1">
         <f>COUNTIF(N9:N1048576,"EMBALAGEM/EXPEDIÇÃO")</f>
         <v>0</v>
       </c>
-      <c r="O5" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="P5" s="7"/>
-      <c r="Q5" s="8"/>
+      <c r="O5" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="P5" s="9"/>
+      <c r="Q5" s="10"/>
       <c r="R5" s="1">
         <f>COUNTIF(N9:N1048576,"FALTA MATERIAL INTERNO / TRANSF")</f>
         <v>0</v>
@@ -699,20 +699,20 @@
     <row r="6" spans="2:20" x14ac:dyDescent="0.25">
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
-      <c r="K6" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="L6" s="7"/>
-      <c r="M6" s="8"/>
+      <c r="K6" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="L6" s="9"/>
+      <c r="M6" s="10"/>
       <c r="N6" s="1">
         <f>COUNTIF(N9:N1048576,"ESPAÇO FÍSICO")</f>
         <v>0</v>
       </c>
-      <c r="O6" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="P6" s="7"/>
-      <c r="Q6" s="8"/>
+      <c r="O6" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="10"/>
       <c r="R6" s="1">
         <f>COUNTIF(N9:N1048576,"FALTA MATERIAL EXTERNO / COMPRAS")</f>
         <v>0</v>
@@ -720,51 +720,52 @@
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="G8" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N8" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="O8" s="7"/>
+      <c r="P8" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q8" s="7"/>
+      <c r="R8" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="S8" s="7"/>
+      <c r="T8" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="N8" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="O8" s="5"/>
-      <c r="P8" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q8" s="5"/>
-      <c r="R8" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="S8" s="5"/>
-      <c r="T8" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="F5:G5"/>
     <mergeCell ref="H5:J5"/>
     <mergeCell ref="B1:T1"/>
     <mergeCell ref="R8:S8"/>
@@ -781,7 +782,6 @@
     <mergeCell ref="K6:M6"/>
     <mergeCell ref="H4:J4"/>
     <mergeCell ref="F4:G4"/>
-    <mergeCell ref="F5:G5"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0.39370078740157483" bottom="0.39370078740157483" header="0.19685039370078741" footer="0.19685039370078741"/>
   <pageSetup paperSize="9" scale="86" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
CORREÇÃO FORMATO META HT
</commit_message>
<xml_diff>
--- a/Producao/Modelos/PROGRAMACAO_PROGRAMACAO_MODELO.xlsx
+++ b/Producao/Modelos/PROGRAMACAO_PROGRAMACAO_MODELO.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CIPOLATTI\SISTEMAS\Producao\Producao\Modelos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC50DD19-09CB-495F-B16C-5D925805548C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBE61F7C-E239-4D9A-93A7-6D0B62935218}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-1110" windowWidth="38640" windowHeight="15720" xr2:uid="{D9A668C6-916A-46D2-B14A-67ECE735CF5F}"/>
+    <workbookView xWindow="38280" yWindow="-15" windowWidth="38640" windowHeight="15720" xr2:uid="{D9A668C6-916A-46D2-B14A-67ECE735CF5F}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -86,9 +86,6 @@
     <t>PENDÊNCIA E/OU OBSERVAÇÃO</t>
   </si>
   <si>
-    <t>PRÓXIMO SETOR</t>
-  </si>
-  <si>
     <t>STATUS</t>
   </si>
   <si>
@@ -105,6 +102,9 @@
   </si>
   <si>
     <t>SETOR:</t>
+  </si>
+  <si>
+    <t>META HT</t>
   </si>
 </sst>
 </file>
@@ -221,7 +221,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -232,6 +232,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -241,17 +247,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -570,7 +576,7 @@
   <dimension ref="B1:T8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5:G5"/>
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -587,6 +593,7 @@
     <col min="12" max="13" width="6.140625" customWidth="1"/>
     <col min="14" max="14" width="8.28515625" customWidth="1"/>
     <col min="15" max="15" width="8.140625" customWidth="1"/>
+    <col min="16" max="16" width="10" customWidth="1"/>
     <col min="17" max="17" width="11.140625" customWidth="1"/>
     <col min="18" max="18" width="10" customWidth="1"/>
     <col min="19" max="19" width="10.85546875" customWidth="1"/>
@@ -594,45 +601,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:20" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="B1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
-      <c r="S1" s="6"/>
-      <c r="T1" s="6"/>
+      <c r="B1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="8"/>
     </row>
     <row r="3" spans="2:20" x14ac:dyDescent="0.25">
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
-      <c r="K3" s="8" t="s">
+      <c r="K3" s="4" t="s">
         <v>1</v>
       </c>
       <c r="L3" s="9"/>
-      <c r="M3" s="10"/>
+      <c r="M3" s="5"/>
       <c r="N3" s="1">
         <f>COUNTIF(N9:N1048576,"FILA/M.O")</f>
         <v>0</v>
       </c>
-      <c r="O3" s="8" t="s">
+      <c r="O3" s="4" t="s">
         <v>5</v>
       </c>
       <c r="P3" s="9"/>
-      <c r="Q3" s="10"/>
+      <c r="Q3" s="5"/>
       <c r="R3" s="1">
         <f>COUNTIF(N9:N1048576,"INDEFINIDO")</f>
         <v>0</v>
@@ -641,27 +648,27 @@
     <row r="4" spans="2:20" x14ac:dyDescent="0.25">
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
-      <c r="F4" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" s="10"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="8" t="s">
+      <c r="F4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="5"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="4" t="s">
         <v>2</v>
       </c>
       <c r="L4" s="9"/>
-      <c r="M4" s="10"/>
+      <c r="M4" s="5"/>
       <c r="N4" s="1">
         <f>COUNTIF(N9:N1048576,"EM ANDAMENTO")</f>
         <v>0</v>
       </c>
-      <c r="O4" s="8" t="s">
+      <c r="O4" s="4" t="s">
         <v>6</v>
       </c>
       <c r="P4" s="9"/>
-      <c r="Q4" s="10"/>
+      <c r="Q4" s="5"/>
       <c r="R4" s="1">
         <f>COUNTIF(N9:N1048576,"PROJETOS")</f>
         <v>0</v>
@@ -670,27 +677,27 @@
     <row r="5" spans="2:20" x14ac:dyDescent="0.25">
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
-      <c r="F5" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5" s="10"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="8" t="s">
+      <c r="F5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="5"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="4" t="s">
         <v>3</v>
       </c>
       <c r="L5" s="9"/>
-      <c r="M5" s="10"/>
+      <c r="M5" s="5"/>
       <c r="N5" s="1">
         <f>COUNTIF(N9:N1048576,"EMBALAGEM/EXPEDIÇÃO")</f>
         <v>0</v>
       </c>
-      <c r="O5" s="8" t="s">
+      <c r="O5" s="4" t="s">
         <v>7</v>
       </c>
       <c r="P5" s="9"/>
-      <c r="Q5" s="10"/>
+      <c r="Q5" s="5"/>
       <c r="R5" s="1">
         <f>COUNTIF(N9:N1048576,"FALTA MATERIAL INTERNO / TRANSF")</f>
         <v>0</v>
@@ -699,20 +706,20 @@
     <row r="6" spans="2:20" x14ac:dyDescent="0.25">
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
-      <c r="K6" s="8" t="s">
+      <c r="K6" s="4" t="s">
         <v>4</v>
       </c>
       <c r="L6" s="9"/>
-      <c r="M6" s="10"/>
+      <c r="M6" s="5"/>
       <c r="N6" s="1">
         <f>COUNTIF(N9:N1048576,"ESPAÇO FÍSICO")</f>
         <v>0</v>
       </c>
-      <c r="O6" s="8" t="s">
+      <c r="O6" s="4" t="s">
         <v>8</v>
       </c>
       <c r="P6" s="9"/>
-      <c r="Q6" s="10"/>
+      <c r="Q6" s="5"/>
       <c r="R6" s="1">
         <f>COUNTIF(N9:N1048576,"FALTA MATERIAL EXTERNO / COMPRAS")</f>
         <v>0</v>
@@ -720,7 +727,7 @@
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>9</v>
@@ -734,44 +741,45 @@
       <c r="F8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="G8" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="11"/>
       <c r="M8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="N8" s="7" t="s">
+      <c r="N8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="O8" s="7"/>
-      <c r="P8" s="7" t="s">
+      <c r="O8" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="Q8" s="7"/>
-      <c r="R8" s="7" t="s">
+      <c r="P8" s="11"/>
+      <c r="Q8" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="S8" s="7"/>
+      <c r="R8" s="11"/>
+      <c r="S8" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="T8" s="1" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="16">
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="Q8:R8"/>
+    <mergeCell ref="O8:P8"/>
+    <mergeCell ref="G8:L8"/>
+    <mergeCell ref="F4:G4"/>
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="H5:J5"/>
     <mergeCell ref="B1:T1"/>
-    <mergeCell ref="R8:S8"/>
-    <mergeCell ref="P8:Q8"/>
-    <mergeCell ref="N8:O8"/>
-    <mergeCell ref="G8:K8"/>
     <mergeCell ref="O3:Q3"/>
     <mergeCell ref="O4:Q4"/>
     <mergeCell ref="O5:Q5"/>
@@ -780,8 +788,6 @@
     <mergeCell ref="K4:M4"/>
     <mergeCell ref="K5:M5"/>
     <mergeCell ref="K6:M6"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="F4:G4"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0.39370078740157483" bottom="0.39370078740157483" header="0.19685039370078741" footer="0.19685039370078741"/>
   <pageSetup paperSize="9" scale="86" orientation="landscape" r:id="rId1"/>

</xml_diff>